<commit_message>
1) Fitting function was changed from equation 9.30 to equation 9.68 from He, Two-Dimensional X-Ray Diffraction (2009). 9.30 does not correctly account for Euler angles.
2) Ability to toggle between solving for 3, 5, and 6 strain components was added, allowing for biaxial, biaxial w/ shear, and full triaxial strain tensors to be solved.
</commit_message>
<xml_diff>
--- a/AdditionalFiles/Defining_D0.xlsx
+++ b/AdditionalFiles/Defining_D0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronwells/ResearchDocuments/Synchrotron_2025.02/Analysis_pyFAI/AdditionalFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E082AD-4588-9A49-AE34-E6E0DBEBD456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EDBF63-290A-9C42-8DAB-5B71F9F733A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35120" yWindow="-8020" windowWidth="30240" windowHeight="17400" xr2:uid="{03764494-1B6D-A14B-B2CF-CE600A4B7EF9}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="29920" windowHeight="17080" xr2:uid="{03764494-1B6D-A14B-B2CF-CE600A4B7EF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Image</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>Color Key</t>
+  </si>
+  <si>
+    <t>From Model - on contour for 0 strain</t>
+  </si>
+  <si>
+    <t>VB-APS-SSAO-6_25C_Map-AO_000288</t>
   </si>
 </sst>
 </file>
@@ -224,7 +230,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -288,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -558,11 +564,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -596,8 +639,8 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -609,15 +652,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -629,7 +663,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -641,6 +675,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1462,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D95AAC-BA5D-674F-AB3D-002BAAA3A2AB}">
-  <dimension ref="B1:L57"/>
+  <dimension ref="B1:L61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="89" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="44.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1505,7 +1562,7 @@
       <c r="J2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="60" t="s">
+      <c r="L2" s="57" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1519,7 +1576,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="15"/>
-      <c r="L3" s="62" t="s">
+      <c r="L3" s="59" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1527,31 +1584,31 @@
       <c r="B4" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="58">
+      <c r="C4" s="55">
         <v>20.264939282242057</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="55">
         <v>27.64763736303799</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="55">
         <v>29.635779011993883</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="55">
         <v>32.575634640320153</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="55">
         <v>33.81674625533298</v>
       </c>
-      <c r="H4" s="58">
+      <c r="H4" s="55">
         <v>35.901909061682005</v>
       </c>
-      <c r="I4" s="58">
+      <c r="I4" s="55">
         <v>40.529880674249931</v>
       </c>
-      <c r="J4" s="59">
+      <c r="J4" s="56">
         <v>44.039205444359553</v>
       </c>
-      <c r="L4" s="63" t="s">
+      <c r="L4" s="60" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1565,22 +1622,22 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="15"/>
-      <c r="L5" s="61" t="s">
+      <c r="L5" s="58" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="48"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="63"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="35" t="s">
@@ -1815,31 +1872,31 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="56">
+      <c r="C15" s="53">
         <v>18.049147999999999</v>
       </c>
-      <c r="D15" s="56">
+      <c r="D15" s="53">
         <v>24.620823000000001</v>
       </c>
-      <c r="E15" s="56">
+      <c r="E15" s="53">
         <v>26.400200999999999</v>
       </c>
-      <c r="F15" s="56">
+      <c r="F15" s="53">
         <v>30.125503999999999</v>
       </c>
-      <c r="G15" s="56">
+      <c r="G15" s="53">
         <v>36.101111000000003</v>
       </c>
-      <c r="H15" s="56">
+      <c r="H15" s="53">
         <v>39.224184999999999</v>
       </c>
-      <c r="I15" s="56">
+      <c r="I15" s="53">
         <v>41.553452999999998</v>
       </c>
-      <c r="J15" s="57">
+      <c r="J15" s="54">
         <v>44.736369000000003</v>
       </c>
     </row>
@@ -1848,35 +1905,35 @@
         <v>35</v>
       </c>
       <c r="C16" s="2">
-        <f>AVERAGE(C7:C15)</f>
+        <f t="shared" ref="C16:J16" si="0">AVERAGE(C7:C15)</f>
         <v>18.050502777777776</v>
       </c>
       <c r="D16" s="2">
-        <f>AVERAGE(D7:D15)</f>
+        <f t="shared" si="0"/>
         <v>24.62080688888889</v>
       </c>
       <c r="E16" s="2">
-        <f>AVERAGE(E7:E15)</f>
+        <f t="shared" si="0"/>
         <v>26.402064111111109</v>
       </c>
       <c r="F16" s="2">
-        <f>AVERAGE(F7:F15)</f>
+        <f t="shared" si="0"/>
         <v>30.12403188888889</v>
       </c>
       <c r="G16" s="2">
-        <f>AVERAGE(G7:G15)</f>
+        <f t="shared" si="0"/>
         <v>36.102668444444447</v>
       </c>
       <c r="H16" s="2">
-        <f>AVERAGE(H7:H15)</f>
+        <f t="shared" si="0"/>
         <v>39.225741888888884</v>
       </c>
       <c r="I16" s="2">
-        <f>AVERAGE(I7:I15)</f>
+        <f t="shared" si="0"/>
         <v>41.563635888888889</v>
       </c>
       <c r="J16" s="16">
-        <f>AVERAGE(J7:J15)</f>
+        <f t="shared" si="0"/>
         <v>44.734026777777778</v>
       </c>
     </row>
@@ -1885,35 +1942,35 @@
         <v>36</v>
       </c>
       <c r="C17" s="3">
-        <f>STDEV(C7:C15)</f>
+        <f t="shared" ref="C17:J17" si="1">STDEV(C7:C15)</f>
         <v>3.2027993528233297E-3</v>
       </c>
       <c r="D17" s="3">
-        <f>STDEV(D7:D15)</f>
+        <f t="shared" si="1"/>
         <v>1.6606039145780217E-3</v>
       </c>
       <c r="E17" s="3">
-        <f>STDEV(E7:E15)</f>
+        <f t="shared" si="1"/>
         <v>1.5607304735643535E-3</v>
       </c>
       <c r="F17" s="3">
-        <f>STDEV(F7:F15)</f>
+        <f t="shared" si="1"/>
         <v>1.9072340210659617E-3</v>
       </c>
       <c r="G17" s="3">
-        <f>STDEV(G7:G15)</f>
+        <f t="shared" si="1"/>
         <v>2.4464651597308207E-3</v>
       </c>
       <c r="H17" s="3">
-        <f>STDEV(H7:H15)</f>
+        <f t="shared" si="1"/>
         <v>1.3215583078744926E-3</v>
       </c>
       <c r="I17" s="3">
-        <f>STDEV(I7:I15)</f>
+        <f t="shared" si="1"/>
         <v>5.0202635748654474E-3</v>
       </c>
       <c r="J17" s="18">
-        <f>STDEV(J7:J15)</f>
+        <f t="shared" si="1"/>
         <v>2.2388083201659052E-3</v>
       </c>
     </row>
@@ -1929,17 +1986,17 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="2:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="48"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="35" t="s">
@@ -2000,31 +2057,31 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="56">
+      <c r="C22" s="53">
         <v>17.960953</v>
       </c>
-      <c r="D22" s="56">
+      <c r="D22" s="53">
         <v>24.498567999999999</v>
       </c>
-      <c r="E22" s="56">
+      <c r="E22" s="53">
         <v>26.266005</v>
       </c>
-      <c r="F22" s="56">
+      <c r="F22" s="53">
         <v>29.973313999999998</v>
       </c>
-      <c r="G22" s="56">
+      <c r="G22" s="53">
         <v>35.924283000000003</v>
       </c>
-      <c r="H22" s="56">
+      <c r="H22" s="53">
         <v>39.033754000000002</v>
       </c>
-      <c r="I22" s="56">
+      <c r="I22" s="53">
         <v>41.351011</v>
       </c>
-      <c r="J22" s="57">
+      <c r="J22" s="54">
         <v>44.510829999999999</v>
       </c>
     </row>
@@ -2037,31 +2094,31 @@
         <v>17.960031333333333</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" ref="D23:J23" si="0">AVERAGE(D20:D22)</f>
+        <f t="shared" ref="D23:J23" si="2">AVERAGE(D20:D22)</f>
         <v>24.499249000000002</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>26.266837999999996</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>29.973106666666666</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>35.923853999999999</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>39.032588999999994</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>41.348611666666663</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44.510221333333334</v>
       </c>
     </row>
@@ -2074,31 +2131,31 @@
         <v>1.9457523823289931E-3</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" ref="D24:J24" si="1">STDEV(D20:D22)</f>
+        <f t="shared" ref="D24:J24" si="3">STDEV(D20:D22)</f>
         <v>8.4025174799110046E-4</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.849141201265439E-4</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0879197274306117E-3</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.460208974968432E-4</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9729771919628639E-3</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.2341981410205149E-3</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9515371719056227E-3</v>
       </c>
     </row>
@@ -2114,17 +2171,17 @@
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="2:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="63"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="39" t="s">
@@ -2337,17 +2394,17 @@
       </c>
     </row>
     <row r="37" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="54"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="51"/>
     </row>
     <row r="38" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
@@ -2358,31 +2415,31 @@
         <v>17.952981399999999</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" ref="D38:J38" si="2">AVERAGE(D27:D37)</f>
+        <f t="shared" ref="D38:J38" si="4">AVERAGE(D27:D37)</f>
         <v>24.496517399999998</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>26.263674600000002</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>29.969442599999997</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>35.923203000000001</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39.031761000000003</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>41.355402400000003</v>
       </c>
       <c r="J38" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44.508421800000001</v>
       </c>
     </row>
@@ -2395,31 +2452,31 @@
         <v>7.6916249453539325E-3</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" ref="D39:J39" si="3">STDEV(D27:D37)</f>
+        <f t="shared" ref="D39:J39" si="5">STDEV(D27:D37)</f>
         <v>5.3664402819752714E-3</v>
       </c>
       <c r="E39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.3473429322828219E-3</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.3781704071871943E-3</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.559273822786849E-3</v>
       </c>
       <c r="H39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.8986834942760875E-3</v>
       </c>
       <c r="I39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.7202920134597222E-3</v>
       </c>
       <c r="J39" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.7724282136778132E-3</v>
       </c>
     </row>
@@ -2435,17 +2492,17 @@
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="2:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="48"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="63"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="39" t="s">
@@ -2777,31 +2834,31 @@
       </c>
     </row>
     <row r="55" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="49" t="s">
+      <c r="B55" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="50">
+      <c r="C55" s="47">
         <v>17.955061000000001</v>
       </c>
-      <c r="D55" s="50">
+      <c r="D55" s="47">
         <v>24.497834999999998</v>
       </c>
-      <c r="E55" s="50">
+      <c r="E55" s="47">
         <v>26.266359999999999</v>
       </c>
-      <c r="F55" s="50">
+      <c r="F55" s="47">
         <v>29.967932999999999</v>
       </c>
-      <c r="G55" s="50">
+      <c r="G55" s="47">
         <v>35.919418999999998</v>
       </c>
-      <c r="H55" s="50">
+      <c r="H55" s="47">
         <v>39.025486000000001</v>
       </c>
-      <c r="I55" s="50">
+      <c r="I55" s="47">
         <v>41.339114000000002</v>
       </c>
-      <c r="J55" s="51">
+      <c r="J55" s="48">
         <v>44.50517</v>
       </c>
     </row>
@@ -2814,31 +2871,31 @@
         <v>17.957429727272725</v>
       </c>
       <c r="D56" s="3">
-        <f t="shared" ref="D56:J56" si="4">AVERAGE(D42:D55)</f>
+        <f t="shared" ref="D56:J56" si="6">AVERAGE(D42:D55)</f>
         <v>24.499119727272728</v>
       </c>
       <c r="E56" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>26.267713545454548</v>
       </c>
       <c r="F56" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>29.972251818181824</v>
       </c>
       <c r="G56" s="3">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(G42:G55)</f>
         <v>35.92393772727273</v>
       </c>
       <c r="H56" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>39.032177454545455</v>
       </c>
       <c r="I56" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>41.355087454545455</v>
       </c>
       <c r="J56" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>44.509847818181818</v>
       </c>
     </row>
@@ -2851,43 +2908,91 @@
         <v>4.3897269867480141E-3</v>
       </c>
       <c r="D57" s="33">
-        <f t="shared" ref="D57:J57" si="5">STDEV(D42:D55)</f>
+        <f t="shared" ref="D57:J57" si="7">STDEV(D42:D55)</f>
         <v>3.3202752021753118E-3</v>
       </c>
       <c r="E57" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.2380287248591393E-3</v>
       </c>
       <c r="F57" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.6585618224214272E-3</v>
       </c>
       <c r="G57" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.2095556608018926E-3</v>
       </c>
       <c r="H57" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.7401335501627024E-3</v>
       </c>
       <c r="I57" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.2511538304417169E-3</v>
       </c>
       <c r="J57" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.745621125289643E-3</v>
       </c>
     </row>
+    <row r="58" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:10" ht="23" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="65"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="65"/>
+      <c r="J59" s="66"/>
+    </row>
+    <row r="60" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="71">
+        <v>17.960905</v>
+      </c>
+      <c r="D60" s="69">
+        <v>24.502082000000001</v>
+      </c>
+      <c r="E60" s="69">
+        <v>26.266745</v>
+      </c>
+      <c r="F60" s="69">
+        <v>29.974326999999999</v>
+      </c>
+      <c r="G60" s="69">
+        <v>35.928975999999999</v>
+      </c>
+      <c r="H60" s="69">
+        <v>39.032336999999998</v>
+      </c>
+      <c r="I60" s="69">
+        <v>41.361823999999999</v>
+      </c>
+      <c r="J60" s="67">
+        <v>44.513362000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C61" s="70"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B26:J26"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B19:J19"/>
     <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B59:J59"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>